<commit_message>
Adding new serial number
</commit_message>
<xml_diff>
--- a/testcases/warranty_defect.xlsx
+++ b/testcases/warranty_defect.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>SerialNumber</t>
   </si>
@@ -22,10 +22,22 @@
     <t>Warranty results</t>
   </si>
   <si>
+    <t>186232441</t>
+  </si>
+  <si>
+    <t>186232437</t>
+  </si>
+  <si>
+    <t>186232440</t>
+  </si>
+  <si>
+    <t>186232442</t>
+  </si>
+  <si>
+    <t>186232438</t>
+  </si>
+  <si>
     <t>186232439</t>
-  </si>
-  <si>
-    <t>186232440</t>
   </si>
   <si>
     <t>We couldn't find a product with this serial number. Please double-check the serial number and try again.</t>
@@ -386,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -408,7 +420,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -419,7 +431,51 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>